<commit_message>
Visualizações R OK e gráficos usuários corrigidos
</commit_message>
<xml_diff>
--- a/dados/experimento_paineis_covid.xlsx
+++ b/dados/experimento_paineis_covid.xlsx
@@ -6,7 +6,9 @@
     <sheet state="visible" name="tabulacao_macro" sheetId="1" r:id="rId4"/>
     <sheet state="visible" name="tabulacao_rgt_categorizacao" sheetId="2" r:id="rId5"/>
   </sheets>
-  <definedNames/>
+  <definedNames>
+    <definedName hidden="1" localSheetId="1" name="_xlnm._FilterDatabase">tabulacao_rgt_categorizacao!$A$1:$BM$13</definedName>
+  </definedNames>
   <calcPr/>
 </workbook>
 </file>
@@ -242,7 +244,7 @@
     <t>O ícone que indica que a página está carregando poderia ser mais pra cima na página, mais visível ao usuário (obs: não visível no topo de tela).</t>
   </si>
   <si>
-    <t>Painel Nacional: Covid-19 (CONASS)</t>
+    <t>Painel Nacional: COVID-19 (CONASS)</t>
   </si>
   <si>
     <t>Achei a apresentação melhor: dá até pra baixar a imagem. Achei mais organizado, apesar do meu “quase erro”, que foi mais falta de atenção.</t>
@@ -2265,7 +2267,7 @@
       <c r="B7" s="3">
         <v>1.0</v>
       </c>
-      <c r="C7" s="4" t="s">
+      <c r="C7" s="7" t="s">
         <v>76</v>
       </c>
       <c r="D7" s="4" t="s">
@@ -3077,7 +3079,7 @@
       <c r="B11" s="3">
         <v>1.0</v>
       </c>
-      <c r="C11" s="4" t="s">
+      <c r="C11" s="7" t="s">
         <v>76</v>
       </c>
       <c r="D11" s="4" t="s">
@@ -5513,7 +5515,7 @@
       <c r="B23" s="3">
         <v>1.0</v>
       </c>
-      <c r="C23" s="4" t="s">
+      <c r="C23" s="7" t="s">
         <v>76</v>
       </c>
       <c r="D23" s="4" t="s">
@@ -5716,7 +5718,7 @@
       <c r="B24" s="3">
         <v>1.0</v>
       </c>
-      <c r="C24" s="4" t="s">
+      <c r="C24" s="7" t="s">
         <v>76</v>
       </c>
       <c r="D24" s="4" t="s">
@@ -5919,7 +5921,7 @@
       <c r="B25" s="3">
         <v>1.0</v>
       </c>
-      <c r="C25" s="4" t="s">
+      <c r="C25" s="7" t="s">
         <v>76</v>
       </c>
       <c r="D25" s="4" t="s">
@@ -6934,7 +6936,7 @@
       <c r="B30" s="3">
         <v>1.0</v>
       </c>
-      <c r="C30" s="4" t="s">
+      <c r="C30" s="7" t="s">
         <v>76</v>
       </c>
       <c r="D30" s="4" t="s">
@@ -8355,7 +8357,7 @@
       <c r="B37" s="3">
         <v>2.0</v>
       </c>
-      <c r="C37" s="4" t="s">
+      <c r="C37" s="7" t="s">
         <v>76</v>
       </c>
       <c r="D37" s="4" t="s">
@@ -9979,7 +9981,7 @@
       <c r="B45" s="3">
         <v>2.0</v>
       </c>
-      <c r="C45" s="4" t="s">
+      <c r="C45" s="7" t="s">
         <v>76</v>
       </c>
       <c r="D45" s="4" t="s">
@@ -11400,7 +11402,7 @@
       <c r="B52" s="3">
         <v>2.0</v>
       </c>
-      <c r="C52" s="4" t="s">
+      <c r="C52" s="7" t="s">
         <v>76</v>
       </c>
       <c r="D52" s="4" t="s">
@@ -11603,7 +11605,7 @@
       <c r="B53" s="3">
         <v>2.0</v>
       </c>
-      <c r="C53" s="4" t="s">
+      <c r="C53" s="7" t="s">
         <v>76</v>
       </c>
       <c r="D53" s="4" t="s">
@@ -12821,7 +12823,7 @@
       <c r="B59" s="3">
         <v>2.0</v>
       </c>
-      <c r="C59" s="4" t="s">
+      <c r="C59" s="7" t="s">
         <v>76</v>
       </c>
       <c r="D59" s="4" t="s">
@@ -14039,7 +14041,7 @@
       <c r="B65" s="3">
         <v>3.0</v>
       </c>
-      <c r="C65" s="4" t="s">
+      <c r="C65" s="7" t="s">
         <v>76</v>
       </c>
       <c r="D65" s="4" t="s">
@@ -14445,7 +14447,7 @@
       <c r="B67" s="3">
         <v>3.0</v>
       </c>
-      <c r="C67" s="4" t="s">
+      <c r="C67" s="7" t="s">
         <v>76</v>
       </c>
       <c r="D67" s="4" t="s">
@@ -14648,7 +14650,7 @@
       <c r="B68" s="3">
         <v>3.0</v>
       </c>
-      <c r="C68" s="4" t="s">
+      <c r="C68" s="7" t="s">
         <v>76</v>
       </c>
       <c r="D68" s="4" t="s">
@@ -14851,7 +14853,7 @@
       <c r="B69" s="3">
         <v>3.0</v>
       </c>
-      <c r="C69" s="4" t="s">
+      <c r="C69" s="7" t="s">
         <v>76</v>
       </c>
       <c r="D69" s="4" t="s">
@@ -18302,7 +18304,7 @@
       <c r="B86" s="3">
         <v>3.0</v>
       </c>
-      <c r="C86" s="4" t="s">
+      <c r="C86" s="7" t="s">
         <v>76</v>
       </c>
       <c r="D86" s="4" t="s">
@@ -21550,7 +21552,7 @@
       <c r="B102" s="3">
         <v>3.0</v>
       </c>
-      <c r="C102" s="4" t="s">
+      <c r="C102" s="7" t="s">
         <v>76</v>
       </c>
       <c r="D102" s="4" t="s">
@@ -21956,7 +21958,7 @@
       <c r="B104" s="3">
         <v>3.0</v>
       </c>
-      <c r="C104" s="4" t="s">
+      <c r="C104" s="7" t="s">
         <v>76</v>
       </c>
       <c r="D104" s="4" t="s">
@@ -22159,7 +22161,7 @@
       <c r="B105" s="3">
         <v>3.0</v>
       </c>
-      <c r="C105" s="4" t="s">
+      <c r="C105" s="7" t="s">
         <v>76</v>
       </c>
       <c r="D105" s="4" t="s">
@@ -24996,6 +24998,9 @@
     </row>
   </sheetData>
   <dataValidations>
+    <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="C2:C118">
+      <formula1>"Coronavírus Brasil (Ministério da Saúde),MonitoraCovid-19 (Fiocruz),Painel Nacional: COVID-19 (CONASS),Brasil.io (iniciativa voluntária)"</formula1>
+    </dataValidation>
     <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="D2:D118">
       <formula1>"Positivo,Negativo"</formula1>
     </dataValidation>
@@ -25004,9 +25009,6 @@
     </dataValidation>
     <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="B2:B118">
       <formula1>"1,2,3"</formula1>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="C2:C118">
-      <formula1>"Coronavírus Brasil (Ministério da Saúde),MonitoraCovid-19 (Fiocruz),Painel Nacional: Covid-19 (CONASS),Brasil.io (iniciativa voluntária)"</formula1>
     </dataValidation>
   </dataValidations>
   <drawing r:id="rId1"/>
@@ -25026,8 +25028,8 @@
   </sheetViews>
   <sheetFormatPr customHeight="1" defaultColWidth="12.63" defaultRowHeight="15.75"/>
   <cols>
-    <col customWidth="1" min="1" max="1" width="4.75"/>
-    <col customWidth="1" min="2" max="2" width="8.63"/>
+    <col customWidth="1" min="1" max="1" width="5.75"/>
+    <col customWidth="1" min="2" max="2" width="10.0"/>
     <col customWidth="1" min="3" max="4" width="22.25"/>
     <col customWidth="1" min="5" max="5" width="34.75"/>
     <col customWidth="1" min="6" max="6" width="13.13"/>
@@ -27607,6 +27609,7 @@
       </c>
     </row>
   </sheetData>
+  <autoFilter ref="$A$1:$BM$13"/>
   <dataValidations>
     <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="F2:BM13">
       <formula1>"TRUE,FALSE"</formula1>

</xml_diff>